<commit_message>
Fix Accounting cus bug
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\workspace\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
   <si>
     <t>Tel : 848 - 62581123   Fax :  848 - 62581129</t>
   </si>
@@ -175,9 +175,6 @@
     <t>PO:</t>
   </si>
   <si>
-    <t>Ten tau:</t>
-  </si>
-  <si>
     <t>BẢNG GHI NỢ - DEBIT NOTE (CUSTOM)</t>
   </si>
   <si>
@@ -289,9 +286,6 @@
     <t>&lt;jx:forEach items="${customFee}" var="custom" varStatus="status"&gt;</t>
   </si>
   <si>
-    <t>${status.index}</t>
-  </si>
-  <si>
     <t>&lt;jx:forEach items="${fee}" var="fe" varStatus="status"&gt;</t>
   </si>
   <si>
@@ -305,6 +299,45 @@
   </si>
   <si>
     <t>HCM, ${updateDate}</t>
+  </si>
+  <si>
+    <t>${bill}</t>
+  </si>
+  <si>
+    <t>Ten tau: ${tentau}</t>
+  </si>
+  <si>
+    <t>${vol}</t>
+  </si>
+  <si>
+    <t>${status.index+1}</t>
+  </si>
+  <si>
+    <t>${cusDecOnNo}</t>
+  </si>
+  <si>
+    <t>${colourApplying}</t>
+  </si>
+  <si>
+    <t>${cusFeeTotal}</t>
+  </si>
+  <si>
+    <t>${cusFeeVat}</t>
+  </si>
+  <si>
+    <t>${cusFinalVal}</t>
+  </si>
+  <si>
+    <t>${chihoTotal}</t>
+  </si>
+  <si>
+    <t>${chihoVat}</t>
+  </si>
+  <si>
+    <t>${total}</t>
+  </si>
+  <si>
+    <t>${chihoFinalVal}</t>
   </si>
 </sst>
 </file>
@@ -627,7 +660,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -725,9 +758,6 @@
     <xf numFmtId="43" fontId="10" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -797,7 +827,48 @@
     <xf numFmtId="43" fontId="20" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -810,12 +881,6 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -831,32 +896,14 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1215,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1311,51 +1358,51 @@
       <c r="M5" s="35"/>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="89" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="89"/>
-      <c r="C6" s="89"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="89"/>
-      <c r="F6" s="89"/>
-      <c r="G6" s="89"/>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="89"/>
-      <c r="L6" s="89"/>
+      <c r="A6" s="80" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="80"/>
+      <c r="G6" s="80"/>
+      <c r="H6" s="80"/>
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="89"/>
-      <c r="B7" s="89"/>
-      <c r="C7" s="89"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="89"/>
-      <c r="I7" s="89"/>
-      <c r="J7" s="89"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="89"/>
+      <c r="A7" s="80"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="80"/>
+      <c r="D7" s="80"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="80"/>
+      <c r="H7" s="80"/>
+      <c r="I7" s="80"/>
+      <c r="J7" s="80"/>
+      <c r="K7" s="80"/>
+      <c r="L7" s="80"/>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="90" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="90"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="90"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
+      <c r="A8" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
@@ -1366,19 +1413,19 @@
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="80" t="s">
-        <v>85</v>
-      </c>
-      <c r="J9" s="80"/>
-      <c r="K9" s="80"/>
-      <c r="L9" s="80"/>
+      <c r="I9" s="92" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="92"/>
+      <c r="K9" s="92"/>
+      <c r="L9" s="92"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
@@ -1390,7 +1437,7 @@
         <v>18</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L10" s="10"/>
     </row>
@@ -1399,7 +1446,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="39"/>
       <c r="D11" s="9"/>
@@ -1411,7 +1458,7 @@
         <v>40</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L11" s="9"/>
     </row>
@@ -1420,7 +1467,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="39"/>
       <c r="D12" s="9"/>
@@ -1432,7 +1479,7 @@
         <v>41</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L12" s="9"/>
     </row>
@@ -1441,15 +1488,15 @@
         <v>15</v>
       </c>
       <c r="B13" s="33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="96" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="96"/>
+      <c r="D13" s="89" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="89"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1460,9 +1507,9 @@
     <row r="14" spans="1:13" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="33"/>
-      <c r="C14" s="59"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="59"/>
+      <c r="E14" s="58"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1474,46 +1521,54 @@
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
+      <c r="B15" s="77" t="s">
+        <v>84</v>
+      </c>
       <c r="C15" s="9" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="39"/>
+      <c r="E15" s="76"/>
       <c r="J15" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="K15" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="K15" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="M15" s="78"/>
+      <c r="M15" s="90"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="37"/>
-      <c r="C16" s="97" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="81" t="s">
+      <c r="B16" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
+      <c r="E16" s="93"/>
+      <c r="F16" s="93"/>
+      <c r="G16" s="3" t="s">
+        <v>89</v>
+      </c>
       <c r="J16" s="9" t="s">
         <v>38</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>77</v>
-      </c>
-      <c r="M16" s="78"/>
+        <v>76</v>
+      </c>
+      <c r="M16" s="90"/>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="34"/>
@@ -1521,8 +1576,10 @@
       <c r="J17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="M17" s="78"/>
+      <c r="K17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="M17" s="90"/>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -1537,46 +1594,46 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="78"/>
+      <c r="M18" s="90"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="84" t="s">
+      <c r="D19" s="94" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="85"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="87" t="s">
+      <c r="E19" s="95"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="82" t="s">
+      <c r="H19" s="87" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="82" t="s">
+      <c r="I19" s="87" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="82" t="s">
+      <c r="J19" s="87" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="82" t="s">
+      <c r="K19" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="82" t="s">
+      <c r="L19" s="87" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="88"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1586,96 +1643,96 @@
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="88"/>
-      <c r="H20" s="83"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
+      <c r="G20" s="98"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="88"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="88"/>
+      <c r="L20" s="88"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="65" t="s">
-        <v>79</v>
-      </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="66"/>
-    </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="B22" s="65" t="s">
+      <c r="A21" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+    </row>
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="78" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="E22" s="60" t="s">
+        <v>61</v>
+      </c>
+      <c r="F22" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="H22" s="62" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="100" t="s">
+        <v>55</v>
+      </c>
+      <c r="J22" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C22" s="65" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="E22" s="61" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="61" t="s">
-        <v>61</v>
-      </c>
-      <c r="G22" s="62" t="s">
-        <v>60</v>
-      </c>
-      <c r="H22" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="I22" s="62" t="s">
+      <c r="K22" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="L22" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="J22" s="64" t="s">
-        <v>66</v>
-      </c>
-      <c r="K22" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="L22" s="61" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="23" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
-      <c r="D23" s="68"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="64"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
+      <c r="A23" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="60"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="60"/>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="69"/>
-      <c r="B24" s="70"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="70"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="73"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="74"/>
-      <c r="K24" s="70"/>
-      <c r="L24" s="70"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="71"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
     </row>
     <row r="25" spans="1:13" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
@@ -1683,22 +1740,28 @@
       <c r="C25" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="59"/>
       <c r="F25" s="47"/>
-      <c r="G25" s="49"/>
+      <c r="G25" s="101" t="s">
+        <v>90</v>
+      </c>
       <c r="H25" s="50"/>
-      <c r="I25" s="51"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="52"/>
-      <c r="L25" s="52"/>
+      <c r="I25" s="101" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" s="101" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="51"/>
+      <c r="L25" s="51"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="92"/>
-      <c r="C26" s="92"/>
+      <c r="B26" s="83"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="42"/>
       <c r="E26" s="42"/>
       <c r="F26" s="42"/>
@@ -1710,114 +1773,120 @@
       <c r="L26" s="43"/>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="64" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="63"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+    </row>
+    <row r="28" spans="1:13" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="79" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="61" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="100" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="64"/>
-      <c r="K27" s="75"/>
-      <c r="L27" s="75"/>
-    </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="61" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="D28" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="68" t="s">
-        <v>70</v>
-      </c>
-      <c r="F28" s="61" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" s="62" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="76" t="s">
-        <v>73</v>
-      </c>
-      <c r="I28" s="62" t="s">
+      <c r="K28" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="J28" s="62" t="s">
-        <v>83</v>
-      </c>
-      <c r="K28" s="64" t="s">
+      <c r="L28" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="L28" s="64" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="68"/>
-      <c r="E29" s="68"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="64"/>
-      <c r="K29" s="75"/>
-      <c r="L29" s="75"/>
-    </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="61"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="64"/>
-      <c r="K30" s="75"/>
-      <c r="L30" s="75"/>
+    </row>
+    <row r="29" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="60"/>
+      <c r="C29" s="60"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="60"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="63"/>
+      <c r="K29" s="74"/>
+      <c r="L29" s="74"/>
+    </row>
+    <row r="30" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="64"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="60"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="74"/>
+      <c r="L30" s="74"/>
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="53" t="s">
+      <c r="A31" s="52"/>
+      <c r="B31" s="53"/>
+      <c r="C31" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="54"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
-      <c r="K31" s="56"/>
-      <c r="L31" s="57"/>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="101" t="s">
+        <v>93</v>
+      </c>
+      <c r="H31" s="55"/>
+      <c r="I31" s="101" t="s">
+        <v>94</v>
+      </c>
+      <c r="J31" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="K31" s="55"/>
+      <c r="L31" s="56"/>
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="93" t="s">
+      <c r="A32" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="94"/>
-      <c r="C32" s="94"/>
-      <c r="D32" s="94"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="95"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="85"/>
+      <c r="D32" s="85"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="86"/>
       <c r="G32" s="46"/>
       <c r="H32" s="44"/>
       <c r="I32" s="46"/>
@@ -1828,18 +1897,18 @@
     <row r="33" spans="1:12" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
-      <c r="C33" s="79"/>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="79"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="79"/>
-      <c r="L33" s="79"/>
-    </row>
-    <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="91"/>
+      <c r="D33" s="91"/>
+      <c r="E33" s="91"/>
+      <c r="F33" s="91"/>
+      <c r="G33" s="91"/>
+      <c r="H33" s="91"/>
+      <c r="I33" s="91"/>
+      <c r="J33" s="91"/>
+      <c r="K33" s="91"/>
+      <c r="L33" s="91"/>
+    </row>
+    <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
         <v>31</v>
       </c>
@@ -1848,15 +1917,17 @@
       <c r="K34" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="77"/>
+      <c r="L34" s="49" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="35" spans="1:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
-      <c r="D35" s="58"/>
+      <c r="B35" s="57"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="57"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="28"/>
@@ -1867,12 +1938,12 @@
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="58" t="s">
+      <c r="A36" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
+      <c r="B36" s="57"/>
+      <c r="C36" s="57"/>
+      <c r="D36" s="57"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="28"/>
@@ -1882,12 +1953,12 @@
       <c r="K36" s="28"/>
     </row>
     <row r="37" spans="1:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="57"/>
+      <c r="D37" s="57"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="28"/>
@@ -1897,12 +1968,12 @@
       <c r="K37" s="28"/>
     </row>
     <row r="38" spans="1:12" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="58" t="s">
+      <c r="A38" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="58"/>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
+      <c r="B38" s="57"/>
+      <c r="C38" s="57"/>
+      <c r="D38" s="57"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="28"/>
@@ -1968,13 +2039,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A6:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="M15:M18"/>
     <mergeCell ref="C33:L33"/>
     <mergeCell ref="I9:L9"/>
@@ -1987,6 +2051,13 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A6:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Update report thong quan
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -752,9 +752,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="10" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -839,6 +836,48 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -860,49 +899,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1358,51 +1358,51 @@
       <c r="M5" s="35"/>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="80" t="s">
+      <c r="A6" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="80"/>
-      <c r="G6" s="80"/>
-      <c r="H6" s="80"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
+      <c r="G6" s="93"/>
+      <c r="H6" s="93"/>
+      <c r="I6" s="93"/>
+      <c r="J6" s="93"/>
+      <c r="K6" s="93"/>
+      <c r="L6" s="93"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="80"/>
-      <c r="B7" s="80"/>
-      <c r="C7" s="80"/>
-      <c r="D7" s="80"/>
-      <c r="E7" s="80"/>
-      <c r="F7" s="80"/>
-      <c r="G7" s="80"/>
-      <c r="H7" s="80"/>
-      <c r="I7" s="80"/>
-      <c r="J7" s="80"/>
-      <c r="K7" s="80"/>
-      <c r="L7" s="80"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="93"/>
+      <c r="C7" s="93"/>
+      <c r="D7" s="93"/>
+      <c r="E7" s="93"/>
+      <c r="F7" s="93"/>
+      <c r="G7" s="93"/>
+      <c r="H7" s="93"/>
+      <c r="I7" s="93"/>
+      <c r="J7" s="93"/>
+      <c r="K7" s="93"/>
+      <c r="L7" s="93"/>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="94" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="81"/>
-      <c r="D8" s="81"/>
-      <c r="E8" s="81"/>
-      <c r="F8" s="81"/>
-      <c r="G8" s="81"/>
-      <c r="H8" s="81"/>
-      <c r="I8" s="81"/>
-      <c r="J8" s="81"/>
-      <c r="K8" s="81"/>
-      <c r="L8" s="81"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
+      <c r="L8" s="94"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
@@ -1413,12 +1413,12 @@
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="92" t="s">
+      <c r="I9" s="84" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="92"/>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1493,10 +1493,10 @@
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="100" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="89"/>
+      <c r="E13" s="100"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1507,9 +1507,9 @@
     <row r="14" spans="1:13" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="33"/>
-      <c r="C14" s="58"/>
+      <c r="C14" s="57"/>
       <c r="D14" s="10"/>
-      <c r="E14" s="58"/>
+      <c r="E14" s="57"/>
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1521,21 +1521,21 @@
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="76" t="s">
         <v>84</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="76"/>
+      <c r="E15" s="75"/>
       <c r="J15" s="9" t="s">
         <v>52</v>
       </c>
       <c r="K15" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="90"/>
+      <c r="M15" s="82"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1547,11 +1547,11 @@
       <c r="C16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="93" t="s">
+      <c r="D16" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="93"/>
-      <c r="F16" s="93"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
       <c r="G16" s="3" t="s">
         <v>89</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="K16" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="M16" s="90"/>
+      <c r="M16" s="82"/>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1579,7 +1579,7 @@
       <c r="K17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="M17" s="90"/>
+      <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -1594,46 +1594,46 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="90"/>
+      <c r="M18" s="82"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="87" t="s">
+      <c r="A19" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="87" t="s">
+      <c r="C19" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="94" t="s">
+      <c r="D19" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="95"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="97" t="s">
+      <c r="E19" s="89"/>
+      <c r="F19" s="90"/>
+      <c r="G19" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="87" t="s">
+      <c r="H19" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="87" t="s">
+      <c r="I19" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="87" t="s">
+      <c r="J19" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="87" t="s">
+      <c r="K19" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="87" t="s">
+      <c r="L19" s="86" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="88"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="88"/>
+      <c r="A20" s="87"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="87"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1643,96 +1643,96 @@
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="98"/>
-      <c r="H20" s="88"/>
-      <c r="I20" s="88"/>
-      <c r="J20" s="88"/>
-      <c r="K20" s="88"/>
-      <c r="L20" s="88"/>
+      <c r="G20" s="92"/>
+      <c r="H20" s="87"/>
+      <c r="I20" s="87"/>
+      <c r="J20" s="87"/>
+      <c r="K20" s="87"/>
+      <c r="L20" s="87"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="64" t="s">
+      <c r="A21" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-    </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="60" t="s">
+      <c r="B21" s="64"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="64"/>
+      <c r="I21" s="64"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="64"/>
+      <c r="L21" s="64"/>
+    </row>
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="78" t="s">
+      <c r="B22" s="77" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="64" t="s">
+      <c r="D22" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="G22" s="61" t="s">
+      <c r="G22" s="60" t="s">
         <v>59</v>
       </c>
-      <c r="H22" s="62" t="s">
+      <c r="H22" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="I22" s="100" t="s">
+      <c r="I22" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="J22" s="99" t="s">
+      <c r="J22" s="79" t="s">
         <v>65</v>
       </c>
-      <c r="K22" s="60" t="s">
+      <c r="K22" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="L22" s="60" t="s">
+      <c r="L22" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
+      <c r="A23" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
     </row>
     <row r="24" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="68"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="71"/>
-      <c r="H24" s="72"/>
-      <c r="I24" s="71"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
+      <c r="A24" s="67"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="70"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="72"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
     </row>
     <row r="25" spans="1:13" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
@@ -1740,28 +1740,28 @@
       <c r="C25" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="59"/>
-      <c r="E25" s="59"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
       <c r="F25" s="47"/>
-      <c r="G25" s="101" t="s">
+      <c r="G25" s="81" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="50"/>
-      <c r="I25" s="101" t="s">
+      <c r="H25" s="49"/>
+      <c r="I25" s="81" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="101" t="s">
+      <c r="J25" s="81" t="s">
         <v>92</v>
       </c>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
+      <c r="K25" s="50"/>
+      <c r="L25" s="50"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="82" t="s">
+      <c r="A26" s="95" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="83"/>
-      <c r="C26" s="83"/>
+      <c r="B26" s="96"/>
+      <c r="C26" s="96"/>
       <c r="D26" s="42"/>
       <c r="E26" s="42"/>
       <c r="F26" s="42"/>
@@ -1773,120 +1773,120 @@
       <c r="L26" s="43"/>
     </row>
     <row r="27" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="64" t="s">
+      <c r="A27" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="75"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
-    </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="60" t="s">
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="66"/>
+      <c r="E27" s="66"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="62"/>
+      <c r="K27" s="73"/>
+      <c r="L27" s="73"/>
+    </row>
+    <row r="28" spans="1:13" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="59" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="79" t="s">
+      <c r="B28" s="78" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="78" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="67" t="s">
+      <c r="D28" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="67" t="s">
+      <c r="E28" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="60" t="s">
+      <c r="F28" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="61" t="s">
+      <c r="G28" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="H28" s="75" t="s">
+      <c r="H28" s="74" t="s">
         <v>72</v>
       </c>
-      <c r="I28" s="100" t="s">
+      <c r="I28" s="80" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="100" t="s">
+      <c r="J28" s="80" t="s">
         <v>81</v>
       </c>
-      <c r="K28" s="63" t="s">
+      <c r="K28" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="L28" s="63" t="s">
+      <c r="L28" s="62" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="64" t="s">
+      <c r="A29" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="75"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="74"/>
-      <c r="L29" s="74"/>
+      <c r="B29" s="59"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="66"/>
+      <c r="E29" s="66"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="62"/>
+      <c r="K29" s="73"/>
+      <c r="L29" s="73"/>
     </row>
     <row r="30" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="64"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="75"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="74"/>
+      <c r="A30" s="63"/>
+      <c r="B30" s="59"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="59"/>
+      <c r="G30" s="60"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="73"/>
+      <c r="L30" s="73"/>
     </row>
     <row r="31" spans="1:13" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="52"/>
-      <c r="B31" s="53"/>
-      <c r="C31" s="52" t="s">
+      <c r="A31" s="51"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="101" t="s">
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="H31" s="55"/>
-      <c r="I31" s="101" t="s">
+      <c r="H31" s="54"/>
+      <c r="I31" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="J31" s="101" t="s">
+      <c r="J31" s="81" t="s">
         <v>96</v>
       </c>
-      <c r="K31" s="55"/>
-      <c r="L31" s="56"/>
+      <c r="K31" s="54"/>
+      <c r="L31" s="55"/>
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="84" t="s">
+      <c r="A32" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="85"/>
-      <c r="C32" s="85"/>
-      <c r="D32" s="85"/>
-      <c r="E32" s="85"/>
-      <c r="F32" s="86"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="98"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="99"/>
       <c r="G32" s="46"/>
       <c r="H32" s="44"/>
       <c r="I32" s="46"/>
@@ -1897,16 +1897,16 @@
     <row r="33" spans="1:12" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="91"/>
-      <c r="F33" s="91"/>
-      <c r="G33" s="91"/>
-      <c r="H33" s="91"/>
-      <c r="I33" s="91"/>
-      <c r="J33" s="91"/>
-      <c r="K33" s="91"/>
-      <c r="L33" s="91"/>
+      <c r="C33" s="83"/>
+      <c r="D33" s="83"/>
+      <c r="E33" s="83"/>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
     </row>
     <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
@@ -1917,17 +1917,17 @@
       <c r="K34" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="49" t="s">
+      <c r="L34" s="101" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="57" t="s">
+      <c r="A35" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="57"/>
-      <c r="C35" s="57"/>
-      <c r="D35" s="57"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="56"/>
+      <c r="D35" s="56"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="28"/>
@@ -1938,12 +1938,12 @@
       <c r="L35" s="13"/>
     </row>
     <row r="36" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="57"/>
-      <c r="D36" s="57"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="28"/>
@@ -1953,12 +1953,12 @@
       <c r="K36" s="28"/>
     </row>
     <row r="37" spans="1:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
       <c r="E37" s="13"/>
       <c r="F37" s="13"/>
       <c r="G37" s="28"/>
@@ -1968,12 +1968,12 @@
       <c r="K37" s="28"/>
     </row>
     <row r="38" spans="1:12" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="13"/>
       <c r="F38" s="13"/>
       <c r="G38" s="28"/>
@@ -2039,6 +2039,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A6:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="M15:M18"/>
     <mergeCell ref="C33:L33"/>
     <mergeCell ref="I9:L9"/>
@@ -2051,13 +2058,6 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A6:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Final version for Debit
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -845,6 +845,39 @@
     <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -857,12 +890,6 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -876,33 +903,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1262,8 +1262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1358,51 +1358,51 @@
       <c r="M5" s="35"/>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="93"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+      <c r="L6" s="83"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="93"/>
-      <c r="B7" s="93"/>
-      <c r="C7" s="93"/>
-      <c r="D7" s="93"/>
-      <c r="E7" s="93"/>
-      <c r="F7" s="93"/>
-      <c r="G7" s="93"/>
-      <c r="H7" s="93"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="93"/>
+      <c r="A7" s="83"/>
+      <c r="B7" s="83"/>
+      <c r="C7" s="83"/>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
+      <c r="A8" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="94"/>
-      <c r="C8" s="94"/>
-      <c r="D8" s="94"/>
-      <c r="E8" s="94"/>
-      <c r="F8" s="94"/>
-      <c r="G8" s="94"/>
-      <c r="H8" s="94"/>
-      <c r="I8" s="94"/>
-      <c r="J8" s="94"/>
-      <c r="K8" s="94"/>
-      <c r="L8" s="94"/>
+      <c r="B8" s="84"/>
+      <c r="C8" s="84"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
@@ -1413,12 +1413,12 @@
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="84" t="s">
+      <c r="I9" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
+      <c r="J9" s="95"/>
+      <c r="K9" s="95"/>
+      <c r="L9" s="95"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1493,10 +1493,10 @@
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="100"/>
+      <c r="E13" s="92"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1535,7 +1535,7 @@
       <c r="K15" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="82"/>
+      <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
@@ -1547,11 +1547,11 @@
       <c r="C16" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="D16" s="85" t="s">
+      <c r="D16" s="96" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="96"/>
       <c r="G16" s="3" t="s">
         <v>89</v>
       </c>
@@ -1561,7 +1561,7 @@
       <c r="K16" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="M16" s="82"/>
+      <c r="M16" s="93"/>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
@@ -1579,7 +1579,7 @@
       <c r="K17" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="M17" s="82"/>
+      <c r="M17" s="93"/>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -1594,46 +1594,46 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="82"/>
+      <c r="M18" s="93"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="86" t="s">
+      <c r="A19" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="86" t="s">
+      <c r="C19" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="88" t="s">
+      <c r="D19" s="97" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="89"/>
-      <c r="F19" s="90"/>
-      <c r="G19" s="91" t="s">
+      <c r="E19" s="98"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="86" t="s">
+      <c r="H19" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="86" t="s">
+      <c r="I19" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="86" t="s">
+      <c r="J19" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="86" t="s">
+      <c r="K19" s="90" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="86" t="s">
+      <c r="L19" s="90" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="87"/>
-      <c r="B20" s="87"/>
-      <c r="C20" s="87"/>
+      <c r="A20" s="91"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="91"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1643,12 +1643,12 @@
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="92"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="87"/>
-      <c r="K20" s="87"/>
-      <c r="L20" s="87"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="91"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="91"/>
+      <c r="K20" s="91"/>
+      <c r="L20" s="91"/>
     </row>
     <row r="21" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="63" t="s">
@@ -1757,11 +1757,11 @@
       <c r="L25" s="50"/>
     </row>
     <row r="26" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="96"/>
-      <c r="C26" s="96"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
       <c r="D26" s="42"/>
       <c r="E26" s="42"/>
       <c r="F26" s="42"/>
@@ -1772,7 +1772,7 @@
       <c r="K26" s="42"/>
       <c r="L26" s="43"/>
     </row>
-    <row r="27" spans="1:13" s="4" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
         <v>79</v>
       </c>
@@ -1879,14 +1879,14 @@
       <c r="L31" s="55"/>
     </row>
     <row r="32" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="97" t="s">
+      <c r="A32" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="98"/>
-      <c r="C32" s="98"/>
-      <c r="D32" s="98"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="99"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="88"/>
+      <c r="D32" s="88"/>
+      <c r="E32" s="88"/>
+      <c r="F32" s="89"/>
       <c r="G32" s="46"/>
       <c r="H32" s="44"/>
       <c r="I32" s="46"/>
@@ -1897,16 +1897,16 @@
     <row r="33" spans="1:12" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
       <c r="B33" s="27"/>
-      <c r="C33" s="83"/>
-      <c r="D33" s="83"/>
-      <c r="E33" s="83"/>
-      <c r="F33" s="83"/>
-      <c r="G33" s="83"/>
-      <c r="H33" s="83"/>
-      <c r="I33" s="83"/>
-      <c r="J33" s="83"/>
-      <c r="K33" s="83"/>
-      <c r="L33" s="83"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="94"/>
+      <c r="E33" s="94"/>
+      <c r="F33" s="94"/>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="94"/>
     </row>
     <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="27" t="s">
@@ -1917,7 +1917,7 @@
       <c r="K34" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="101" t="s">
+      <c r="L34" s="82" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2039,13 +2039,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A6:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="M15:M18"/>
     <mergeCell ref="C33:L33"/>
     <mergeCell ref="I9:L9"/>
@@ -2058,6 +2051,13 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A6:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
- update report template
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="117" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" calcMode="manual"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
   <si>
     <t>Tel : 848 - 62581123   Fax :  848 - 62581129</t>
   </si>
@@ -211,90 +211,15 @@
     <t>${noOfPkgs}</t>
   </si>
   <si>
-    <t>&lt;/jx:forEach&gt;</t>
-  </si>
-  <si>
-    <t>${custom.feevat}</t>
-  </si>
-  <si>
-    <t>${custom.invoice}</t>
-  </si>
-  <si>
-    <t>${custom.note}</t>
-  </si>
-  <si>
-    <t>${custom.vat}</t>
-  </si>
-  <si>
-    <t>${custom.total}</t>
-  </si>
-  <si>
-    <t>${custom.numOfLCL}</t>
-  </si>
-  <si>
-    <t>${custom.numOf40}</t>
-  </si>
-  <si>
-    <t>${custom.numOf20}</t>
-  </si>
-  <si>
-    <t>${custom.feeDescription}</t>
-  </si>
-  <si>
-    <t>${custom.feeName}</t>
-  </si>
-  <si>
-    <t>${custom.feewithvat}</t>
-  </si>
-  <si>
-    <t>${fe.feeName}</t>
-  </si>
-  <si>
-    <t>${fe.feeDescription}</t>
-  </si>
-  <si>
-    <t>${fe.numOf20}</t>
-  </si>
-  <si>
-    <t>${fe.numOf40}</t>
-  </si>
-  <si>
-    <t>${fe.numOfLCL}</t>
-  </si>
-  <si>
-    <t>${fe.total}</t>
-  </si>
-  <si>
-    <t>${fe.vat}</t>
-  </si>
-  <si>
-    <t>${fe.feevat}</t>
-  </si>
-  <si>
-    <t>${fe.note}</t>
-  </si>
-  <si>
-    <t>${fe.invoice}</t>
-  </si>
-  <si>
     <t>${kg}</t>
   </si>
   <si>
     <t>${placeDelivery}</t>
   </si>
   <si>
-    <t>&lt;jx:forEach items="${customFee}" var="custom" varStatus="status"&gt;</t>
-  </si>
-  <si>
-    <t>&lt;jx:forEach items="${fee}" var="fe" varStatus="status"&gt;</t>
-  </si>
-  <si>
     <t>Số : ${refNo}</t>
   </si>
   <si>
-    <t>${fe.feewithvat}</t>
-  </si>
-  <si>
     <t>Ngày: ${updateDate}</t>
   </si>
   <si>
@@ -310,9 +235,6 @@
     <t>${vol}</t>
   </si>
   <si>
-    <t>${status.index+1}</t>
-  </si>
-  <si>
     <t>${cusDecOnNo}</t>
   </si>
   <si>
@@ -338,6 +260,78 @@
   </si>
   <si>
     <t>${chihoFinalVal}</t>
+  </si>
+  <si>
+    <t>${customFees.feeName}</t>
+  </si>
+  <si>
+    <t>${customFees.feeDescription}</t>
+  </si>
+  <si>
+    <t>${customFees.numOf20}</t>
+  </si>
+  <si>
+    <t>${customFees.numOf40}</t>
+  </si>
+  <si>
+    <t>${customFees.numOfLCL}</t>
+  </si>
+  <si>
+    <t>${customFees.total}</t>
+  </si>
+  <si>
+    <t>${customFees.vat}</t>
+  </si>
+  <si>
+    <t>${customFees.feevat}</t>
+  </si>
+  <si>
+    <t>${customFees.feewithvat}</t>
+  </si>
+  <si>
+    <t>${customFees.note}</t>
+  </si>
+  <si>
+    <t>${customFees.invoice}</t>
+  </si>
+  <si>
+    <t>${fees.feeName}</t>
+  </si>
+  <si>
+    <t>${fees.feeDescription}</t>
+  </si>
+  <si>
+    <t>${fees.numOf20}</t>
+  </si>
+  <si>
+    <t>${fees.numOf40}</t>
+  </si>
+  <si>
+    <t>${fees.numOfLCL}</t>
+  </si>
+  <si>
+    <t>${fees.total}</t>
+  </si>
+  <si>
+    <t>${fees.vat}</t>
+  </si>
+  <si>
+    <t>${fees.feevat}</t>
+  </si>
+  <si>
+    <t>${fees.feewithvat}</t>
+  </si>
+  <si>
+    <t>${fees.note}</t>
+  </si>
+  <si>
+    <t>${fees.invoice}</t>
+  </si>
+  <si>
+    <t>${customFees.index}</t>
+  </si>
+  <si>
+    <t>${fees.index}</t>
   </si>
 </sst>
 </file>
@@ -350,7 +344,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -520,20 +514,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -660,7 +640,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -791,36 +771,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="7" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="43" fontId="20" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -848,6 +798,39 @@
     <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -869,41 +852,8 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1260,10 +1210,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1358,51 +1308,51 @@
       <c r="M5" s="35"/>
     </row>
     <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
+      <c r="A6" s="84" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="83"/>
-      <c r="C6" s="83"/>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="84"/>
+      <c r="D6" s="84"/>
+      <c r="E6" s="84"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="84"/>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84"/>
+      <c r="J6" s="84"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="84"/>
       <c r="M6" s="36"/>
     </row>
     <row r="7" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="83"/>
-      <c r="C7" s="83"/>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
+      <c r="A7" s="84"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="84"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="84"/>
+      <c r="J7" s="84"/>
+      <c r="K7" s="84"/>
+      <c r="L7" s="84"/>
     </row>
     <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="84" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
+      <c r="A8" s="85" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="85"/>
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
     </row>
     <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
@@ -1413,12 +1363,12 @@
       <c r="F9" s="38"/>
       <c r="G9" s="38"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="95" t="s">
-        <v>83</v>
-      </c>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
+      <c r="I9" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -1493,10 +1443,10 @@
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="92" t="s">
+      <c r="D13" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="92"/>
+      <c r="E13" s="91"/>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
@@ -1521,54 +1471,54 @@
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="76" t="s">
-        <v>84</v>
+      <c r="B15" s="66" t="s">
+        <v>59</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="75"/>
+      <c r="E15" s="65"/>
       <c r="J15" s="9" t="s">
         <v>52</v>
       </c>
       <c r="K15" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="93"/>
+      <c r="M15" s="73"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" s="96" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="96"/>
-      <c r="F16" s="96"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
       <c r="G16" s="3" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="J16" s="9" t="s">
         <v>38</v>
       </c>
       <c r="K16" s="33" t="s">
-        <v>76</v>
-      </c>
-      <c r="M16" s="93"/>
+        <v>54</v>
+      </c>
+      <c r="M16" s="73"/>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="34"/>
@@ -1577,9 +1527,9 @@
         <v>39</v>
       </c>
       <c r="K17" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="M17" s="93"/>
+        <v>61</v>
+      </c>
+      <c r="M17" s="73"/>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
@@ -1594,46 +1544,46 @@
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="32"/>
-      <c r="M18" s="93"/>
+      <c r="M18" s="73"/>
     </row>
     <row r="19" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="90" t="s">
+      <c r="A19" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="90" t="s">
+      <c r="B19" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="90" t="s">
+      <c r="C19" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="97" t="s">
+      <c r="D19" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="98"/>
-      <c r="F19" s="99"/>
-      <c r="G19" s="100" t="s">
+      <c r="E19" s="80"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="90" t="s">
+      <c r="H19" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="90" t="s">
+      <c r="I19" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="90" t="s">
+      <c r="J19" s="77" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="90" t="s">
+      <c r="K19" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="90" t="s">
+      <c r="L19" s="77" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="91"/>
-      <c r="B20" s="91"/>
-      <c r="C20" s="91"/>
+      <c r="A20" s="78"/>
+      <c r="B20" s="78"/>
+      <c r="C20" s="78"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1643,404 +1593,319 @@
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="101"/>
-      <c r="H20" s="91"/>
-      <c r="I20" s="91"/>
-      <c r="J20" s="91"/>
-      <c r="K20" s="91"/>
-      <c r="L20" s="91"/>
-    </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="s">
+      <c r="G20" s="83"/>
+      <c r="H20" s="78"/>
+      <c r="I20" s="78"/>
+      <c r="J20" s="78"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="78"/>
+    </row>
+    <row r="21" spans="1:13" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="67" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" s="59" t="s">
+        <v>75</v>
+      </c>
+      <c r="G21" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="H21" s="61" t="s">
+        <v>77</v>
+      </c>
+      <c r="I21" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-    </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="59" t="s">
+      <c r="J21" s="69" t="s">
+        <v>79</v>
+      </c>
+      <c r="K21" s="59" t="s">
+        <v>80</v>
+      </c>
+      <c r="L21" s="59" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="H22" s="49"/>
+      <c r="I22" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="J22" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="K22" s="50"/>
+      <c r="L22" s="50"/>
+    </row>
+    <row r="23" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="86" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="87"/>
+      <c r="C23" s="87"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="43"/>
+    </row>
+    <row r="24" spans="1:13" s="4" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="68" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="59" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="60" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="77" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="77" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" s="63" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" s="59" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="G22" s="60" t="s">
-        <v>59</v>
-      </c>
-      <c r="H22" s="61" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="80" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" s="79" t="s">
-        <v>65</v>
-      </c>
-      <c r="K22" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="L22" s="59" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="59"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="59"/>
-    </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="67"/>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="68"/>
-      <c r="G24" s="70"/>
-      <c r="H24" s="71"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="72"/>
-      <c r="K24" s="68"/>
-      <c r="L24" s="68"/>
-    </row>
-    <row r="25" spans="1:13" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="47"/>
-      <c r="C25" s="48" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="58"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="81" t="s">
+      <c r="H24" s="64" t="s">
+        <v>88</v>
+      </c>
+      <c r="I24" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="49"/>
-      <c r="I25" s="81" t="s">
+      <c r="K24" s="62" t="s">
         <v>91</v>
       </c>
-      <c r="J25" s="81" t="s">
+      <c r="L24" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="K25" s="50"/>
-      <c r="L25" s="50"/>
-    </row>
-    <row r="26" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="85" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="86"/>
-      <c r="C26" s="86"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="L26" s="43"/>
-    </row>
-    <row r="27" spans="1:13" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="60"/>
+    </row>
+    <row r="25" spans="1:13" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="51"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="71" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25" s="54"/>
+      <c r="I25" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="J25" s="71" t="s">
+        <v>70</v>
+      </c>
+      <c r="K25" s="54"/>
+      <c r="L25" s="55"/>
+    </row>
+    <row r="26" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="88" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="89"/>
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="90"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
+    </row>
+    <row r="27" spans="1:13" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="27"/>
+      <c r="C27" s="74"/>
+      <c r="D27" s="74"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
       <c r="H27" s="74"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="73"/>
-      <c r="L27" s="73"/>
-    </row>
-    <row r="28" spans="1:13" s="4" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="78" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="78" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="66" t="s">
-        <v>68</v>
-      </c>
-      <c r="E28" s="66" t="s">
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
+      <c r="K27" s="74"/>
+      <c r="L27" s="74"/>
+    </row>
+    <row r="28" spans="1:13" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="27"/>
+      <c r="D28" s="20"/>
+      <c r="K28" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="L28" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="F28" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="60" t="s">
-        <v>71</v>
-      </c>
-      <c r="H28" s="74" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" s="80" t="s">
-        <v>73</v>
-      </c>
-      <c r="J28" s="80" t="s">
-        <v>81</v>
-      </c>
-      <c r="K28" s="62" t="s">
-        <v>74</v>
-      </c>
-      <c r="L28" s="62" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="59"/>
-      <c r="C29" s="59"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="59"/>
-      <c r="G29" s="60"/>
-      <c r="H29" s="74"/>
-      <c r="I29" s="60"/>
-      <c r="J29" s="62"/>
-      <c r="K29" s="73"/>
-      <c r="L29" s="73"/>
-    </row>
-    <row r="30" spans="1:13" s="4" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="63"/>
-      <c r="B30" s="59"/>
-      <c r="C30" s="59"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="59"/>
-      <c r="G30" s="60"/>
-      <c r="H30" s="74"/>
-      <c r="I30" s="60"/>
-      <c r="J30" s="62"/>
-      <c r="K30" s="73"/>
-      <c r="L30" s="73"/>
-    </row>
-    <row r="31" spans="1:13" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="H31" s="54"/>
-      <c r="I31" s="81" t="s">
-        <v>94</v>
-      </c>
-      <c r="J31" s="81" t="s">
-        <v>96</v>
-      </c>
-      <c r="K31" s="54"/>
-      <c r="L31" s="55"/>
-    </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="87" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="88"/>
-      <c r="C32" s="88"/>
-      <c r="D32" s="88"/>
-      <c r="E32" s="88"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="46"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="46"/>
-      <c r="J32" s="46"/>
-      <c r="K32" s="44"/>
-      <c r="L32" s="44"/>
-    </row>
-    <row r="33" spans="1:12" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="27"/>
-      <c r="B33" s="27"/>
-      <c r="C33" s="94"/>
-      <c r="D33" s="94"/>
-      <c r="E33" s="94"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="94"/>
-      <c r="H33" s="94"/>
-      <c r="I33" s="94"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="94"/>
-      <c r="L33" s="94"/>
-    </row>
-    <row r="34" spans="1:12" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="27"/>
-      <c r="D34" s="20"/>
-      <c r="K34" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="L34" s="82" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="56" t="s">
+    </row>
+    <row r="29" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="56"/>
-      <c r="C35" s="56"/>
-      <c r="D35" s="56"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
-      <c r="L35" s="13"/>
-    </row>
-    <row r="36" spans="1:12" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="28"/>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="13"/>
+    </row>
+    <row r="30" spans="1:13" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="56"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="56"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="28"/>
-      <c r="H36" s="28"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="28"/>
-      <c r="K36" s="28"/>
-    </row>
-    <row r="37" spans="1:12" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="56" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="28"/>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+    </row>
+    <row r="31" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="56"/>
-      <c r="C37" s="56"/>
-      <c r="D37" s="56"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-    </row>
-    <row r="38" spans="1:12" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="56" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="28"/>
+      <c r="H31" s="28"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+    </row>
+    <row r="32" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="56" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="56"/>
-      <c r="C38" s="56"/>
-      <c r="D38" s="56"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="28"/>
-      <c r="H38" s="28"/>
-      <c r="I38" s="28"/>
-      <c r="J38" s="29"/>
-      <c r="K38" s="29"/>
-    </row>
-    <row r="39" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="22"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="22"/>
-      <c r="I39" s="22"/>
-      <c r="J39" s="22"/>
-      <c r="K39" s="22"/>
-    </row>
-    <row r="40" spans="1:12" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="22"/>
-      <c r="D40" s="22"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="22"/>
-      <c r="I40" s="22"/>
-      <c r="J40" s="22"/>
-      <c r="K40" s="22"/>
-    </row>
-    <row r="41" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="31" t="s">
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+    </row>
+    <row r="33" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="30"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+    </row>
+    <row r="34" spans="1:12" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="30"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+    </row>
+    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B41" s="31"/>
-      <c r="C41" s="22"/>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="31" t="s">
+      <c r="B35" s="31"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="22"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+    </row>
+    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="1"/>
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="1"/>
-    </row>
-    <row r="48" spans="1:12" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="12:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L52" s="21"/>
-    </row>
-    <row r="61" spans="12:12" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="65" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C65" s="15"/>
+      <c r="L46" s="21"/>
+    </row>
+    <row r="55" spans="3:3" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A6:L7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D13:E13"/>
     <mergeCell ref="M15:M18"/>
-    <mergeCell ref="C33:L33"/>
+    <mergeCell ref="C27:L27"/>
     <mergeCell ref="I9:L9"/>
     <mergeCell ref="D16:F16"/>
     <mergeCell ref="C19:C20"/>
@@ -2051,13 +1916,6 @@
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A6:L7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
+ Cho thêm 1 cột đơn giá (nhân với số lượng để thành tiền) Nếu nhập giá trị vào đơn giá thì disable change trong field thành tiền. Nếu cột đơn giá không có giá trị thì cho nhập trong thành tiền. + Thêm giá trị cho dropdown "Mô tả dịch vụ" (related to General issue)
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="117" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t>Tel : 848 - 62581123   Fax :  848 - 62581129</t>
   </si>
@@ -332,6 +332,12 @@
   </si>
   <si>
     <t>${fees.index}</t>
+  </si>
+  <si>
+    <t>Đơn Giá</t>
+  </si>
+  <si>
+    <t>${customFees.unitPrice}</t>
   </si>
 </sst>
 </file>
@@ -640,7 +646,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -759,21 +765,12 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="20" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="20" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -786,17 +783,50 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -810,12 +840,6 @@
     <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -831,29 +855,26 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="4" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1210,167 +1231,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M59"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="17" customWidth="1"/>
-    <col min="5" max="6" width="5.85546875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="16" style="2" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="14.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" style="17" customWidth="1"/>
+    <col min="5" max="7" width="5.81640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="12.453125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="14.7265625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.453125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16" style="2" customWidth="1"/>
+    <col min="14" max="14" width="21.1796875" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G1" s="22"/>
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="H1" s="22"/>
-      <c r="L1" s="40" t="s">
+      <c r="I1" s="22"/>
+      <c r="M1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="23"/>
-    </row>
-    <row r="2" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N1" s="23"/>
+    </row>
+    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="18"/>
       <c r="E2" s="6"/>
       <c r="F2" s="7"/>
-      <c r="G2" s="24"/>
+      <c r="G2" s="7"/>
       <c r="H2" s="24"/>
-      <c r="I2" s="7"/>
+      <c r="I2" s="24"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="7"/>
+      <c r="M2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N2" s="25"/>
+    </row>
+    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="18"/>
       <c r="E3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="G3" s="24"/>
+      <c r="G3" s="7"/>
       <c r="H3" s="24"/>
-      <c r="I3" s="7"/>
+      <c r="I3" s="24"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="7"/>
+      <c r="M3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="25"/>
-    </row>
-    <row r="4" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="25"/>
+    </row>
+    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="18"/>
       <c r="E4" s="6"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="24"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="24"/>
-      <c r="I4" s="7"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="7"/>
+      <c r="M4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="25"/>
-    </row>
-    <row r="5" spans="1:13" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N4" s="25"/>
+    </row>
+    <row r="5" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
       <c r="D5" s="19"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="26"/>
+      <c r="G5" s="14"/>
       <c r="H5" s="26"/>
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
-      <c r="M5" s="35"/>
-    </row>
-    <row r="6" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="84" t="s">
+      <c r="M5" s="26"/>
+      <c r="N5" s="35"/>
+    </row>
+    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="36"/>
-    </row>
-    <row r="7" spans="1:13" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="84"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-    </row>
-    <row r="8" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="85" t="s">
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="71"/>
+      <c r="K6" s="71"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="71"/>
+      <c r="N6" s="36"/>
+    </row>
+    <row r="7" spans="1:14" ht="2.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="71"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="71"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="71"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
+      <c r="L7" s="71"/>
+      <c r="M7" s="71"/>
+    </row>
+    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="85"/>
-      <c r="C8" s="85"/>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
-      <c r="F8" s="85"/>
-      <c r="G8" s="85"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-    </row>
-    <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
+      <c r="H8" s="72"/>
+      <c r="I8" s="72"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+    </row>
+    <row r="9" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
       <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="68"/>
       <c r="H9" s="38"/>
-      <c r="I9" s="75" t="s">
+      <c r="I9" s="38"/>
+      <c r="J9" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="J9" s="75"/>
-      <c r="K9" s="75"/>
-      <c r="L9" s="75"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+    </row>
+    <row r="10" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1380,18 +1409,18 @@
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
-      <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="L10" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1401,18 +1430,18 @@
       <c r="C11" s="39"/>
       <c r="D11" s="9"/>
       <c r="E11" s="39"/>
-      <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="L11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="L11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1422,18 +1451,18 @@
       <c r="C12" s="39"/>
       <c r="D12" s="9"/>
       <c r="E12" s="39"/>
-      <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="L12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1443,51 +1472,51 @@
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="80" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="91"/>
-      <c r="G13" s="9"/>
+      <c r="E13" s="80"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8"/>
       <c r="B14" s="33"/>
       <c r="C14" s="57"/>
       <c r="D14" s="10"/>
       <c r="E14" s="57"/>
-      <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="66" t="s">
+      <c r="B15" s="63" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>60</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="65"/>
-      <c r="J15" s="9" t="s">
+      <c r="E15" s="62"/>
+      <c r="K15" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="33" t="s">
+      <c r="L15" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="73"/>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N15" s="81"/>
+    </row>
+    <row r="16" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
@@ -1497,23 +1526,24 @@
       <c r="C16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="76" t="s">
+      <c r="D16" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="3" t="s">
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="67"/>
+      <c r="H16" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="K16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="33" t="s">
+      <c r="L16" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="M16" s="73"/>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N16" s="81"/>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>43</v>
       </c>
@@ -1523,67 +1553,71 @@
       <c r="C17" s="16"/>
       <c r="D17" s="34"/>
       <c r="E17" s="39"/>
-      <c r="J17" s="9" t="s">
+      <c r="K17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="L17" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="M17" s="73"/>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N17" s="81"/>
+    </row>
+    <row r="18" spans="1:14" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
       <c r="E18" s="9"/>
       <c r="F18" s="39"/>
-      <c r="G18" s="9"/>
+      <c r="G18" s="66"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-      <c r="L18" s="32"/>
-      <c r="M18" s="73"/>
-    </row>
-    <row r="19" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="77" t="s">
+      <c r="L18" s="9"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="81"/>
+    </row>
+    <row r="19" spans="1:14" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="77" t="s">
+      <c r="B19" s="78" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="79" t="s">
+      <c r="D19" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="80"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="82" t="s">
+      <c r="E19" s="86"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="90" t="s">
+        <v>95</v>
+      </c>
+      <c r="H19" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="77" t="s">
+      <c r="I19" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="77" t="s">
+      <c r="J19" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="J19" s="77" t="s">
+      <c r="K19" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="K19" s="77" t="s">
+      <c r="L19" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="L19" s="77" t="s">
+      <c r="M19" s="78" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="78"/>
-      <c r="B20" s="78"/>
-      <c r="C20" s="78"/>
+    <row r="20" spans="1:14" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="79"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="79"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1593,24 +1627,25 @@
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="83"/>
-      <c r="H20" s="78"/>
-      <c r="I20" s="78"/>
-      <c r="J20" s="78"/>
-      <c r="K20" s="78"/>
-      <c r="L20" s="78"/>
-    </row>
-    <row r="21" spans="1:13" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="67" t="s">
+      <c r="G20" s="91"/>
+      <c r="H20" s="89"/>
+      <c r="I20" s="79"/>
+      <c r="J20" s="79"/>
+      <c r="K20" s="79"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="79"/>
+    </row>
+    <row r="21" spans="1:14" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="67" t="s">
+      <c r="B21" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="67" t="s">
+      <c r="C21" s="64" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="61" t="s">
         <v>73</v>
       </c>
       <c r="E21" s="59" t="s">
@@ -1619,26 +1654,29 @@
       <c r="F21" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="60" t="s">
+      <c r="G21" s="92" t="s">
+        <v>96</v>
+      </c>
+      <c r="H21" s="93" t="s">
         <v>76</v>
       </c>
-      <c r="H21" s="61" t="s">
+      <c r="I21" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="I21" s="70" t="s">
+      <c r="J21" s="93" t="s">
         <v>78</v>
       </c>
-      <c r="J21" s="69" t="s">
+      <c r="K21" s="92" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="59" t="s">
+      <c r="L21" s="59" t="s">
         <v>80</v>
       </c>
-      <c r="L21" s="59" t="s">
+      <c r="M21" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="47"/>
       <c r="B22" s="47"/>
       <c r="C22" s="48" t="s">
@@ -1647,25 +1685,26 @@
       <c r="D22" s="58"/>
       <c r="E22" s="58"/>
       <c r="F22" s="47"/>
-      <c r="G22" s="71" t="s">
+      <c r="G22" s="47"/>
+      <c r="H22" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="H22" s="49"/>
-      <c r="I22" s="71" t="s">
+      <c r="I22" s="49"/>
+      <c r="J22" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="J22" s="71" t="s">
+      <c r="K22" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="K22" s="50"/>
       <c r="L22" s="50"/>
-    </row>
-    <row r="23" spans="1:13" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="86" t="s">
+      <c r="M22" s="50"/>
+    </row>
+    <row r="23" spans="1:14" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="87"/>
-      <c r="C23" s="87"/>
+      <c r="B23" s="74"/>
+      <c r="C23" s="74"/>
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
@@ -1674,16 +1713,17 @@
       <c r="I23" s="42"/>
       <c r="J23" s="42"/>
       <c r="K23" s="42"/>
-      <c r="L23" s="43"/>
-    </row>
-    <row r="24" spans="1:13" s="4" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+      <c r="L23" s="42"/>
+      <c r="M23" s="43"/>
+    </row>
+    <row r="24" spans="1:14" s="4" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="64" t="s">
         <v>94</v>
       </c>
-      <c r="B24" s="68" t="s">
+      <c r="B24" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="68" t="s">
+      <c r="C24" s="65" t="s">
         <v>83</v>
       </c>
       <c r="D24" s="59" t="s">
@@ -1695,26 +1735,27 @@
       <c r="F24" s="59" t="s">
         <v>86</v>
       </c>
-      <c r="G24" s="60" t="s">
+      <c r="G24" s="59"/>
+      <c r="H24" s="93" t="s">
         <v>87</v>
       </c>
-      <c r="H24" s="64" t="s">
+      <c r="I24" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="I24" s="70" t="s">
+      <c r="J24" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="J24" s="70" t="s">
+      <c r="K24" s="93" t="s">
         <v>90</v>
       </c>
-      <c r="K24" s="62" t="s">
+      <c r="L24" s="60" t="s">
         <v>91</v>
       </c>
-      <c r="L24" s="62" t="s">
+      <c r="M24" s="60" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="51"/>
       <c r="B25" s="52"/>
       <c r="C25" s="51" t="s">
@@ -1723,63 +1764,66 @@
       <c r="D25" s="52"/>
       <c r="E25" s="52"/>
       <c r="F25" s="53"/>
-      <c r="G25" s="71" t="s">
+      <c r="G25" s="70"/>
+      <c r="H25" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="H25" s="54"/>
-      <c r="I25" s="71" t="s">
+      <c r="I25" s="54"/>
+      <c r="J25" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="J25" s="71" t="s">
+      <c r="K25" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="55"/>
-    </row>
-    <row r="26" spans="1:13" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="88" t="s">
+      <c r="L25" s="54"/>
+      <c r="M25" s="55"/>
+    </row>
+    <row r="26" spans="1:14" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="75" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="89"/>
-      <c r="C26" s="89"/>
-      <c r="D26" s="89"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="90"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="46"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="76"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="76"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="44"/>
       <c r="J26" s="46"/>
-      <c r="K26" s="44"/>
+      <c r="K26" s="46"/>
       <c r="L26" s="44"/>
-    </row>
-    <row r="27" spans="1:13" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M26" s="44"/>
+    </row>
+    <row r="27" spans="1:14" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74"/>
-      <c r="H27" s="74"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="74"/>
-      <c r="K27" s="74"/>
-      <c r="L27" s="74"/>
-    </row>
-    <row r="28" spans="1:13" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+    </row>
+    <row r="28" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="27"/>
       <c r="D28" s="20"/>
-      <c r="K28" s="45" t="s">
+      <c r="L28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="L28" s="72" t="s">
+      <c r="M28" s="96" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="56" t="s">
         <v>32</v>
       </c>
@@ -1788,14 +1832,15 @@
       <c r="D29" s="56"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
-      <c r="G29" s="28"/>
+      <c r="G29" s="13"/>
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
       <c r="J29" s="28"/>
       <c r="K29" s="28"/>
-      <c r="L29" s="13"/>
-    </row>
-    <row r="30" spans="1:13" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L29" s="28"/>
+      <c r="M29" s="13"/>
+    </row>
+    <row r="30" spans="1:14" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="56" t="s">
         <v>33</v>
       </c>
@@ -1804,13 +1849,14 @@
       <c r="D30" s="56"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
-      <c r="G30" s="28"/>
+      <c r="G30" s="13"/>
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
-    </row>
-    <row r="31" spans="1:13" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L30" s="28"/>
+    </row>
+    <row r="31" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="56" t="s">
         <v>34</v>
       </c>
@@ -1819,13 +1865,14 @@
       <c r="D31" s="56"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
-      <c r="G31" s="28"/>
+      <c r="G31" s="13"/>
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
       <c r="K31" s="28"/>
-    </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L31" s="28"/>
+    </row>
+    <row r="32" spans="1:14" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="56" t="s">
         <v>35</v>
       </c>
@@ -1834,13 +1881,14 @@
       <c r="D32" s="56"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
-      <c r="G32" s="28"/>
+      <c r="G32" s="13"/>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
-      <c r="J32" s="29"/>
+      <c r="J32" s="28"/>
       <c r="K32" s="29"/>
-    </row>
-    <row r="33" spans="1:12" ht="3" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L32" s="29"/>
+    </row>
+    <row r="33" spans="1:13" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="22"/>
@@ -1852,8 +1900,9 @@
       <c r="I33" s="22"/>
       <c r="J33" s="22"/>
       <c r="K33" s="22"/>
-    </row>
-    <row r="34" spans="1:12" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L33" s="22"/>
+    </row>
+    <row r="34" spans="1:13" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="22"/>
@@ -1865,8 +1914,9 @@
       <c r="I34" s="22"/>
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
-    </row>
-    <row r="35" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L34" s="22"/>
+    </row>
+    <row r="35" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A35" s="31" t="s">
         <v>7</v>
       </c>
@@ -1875,47 +1925,49 @@
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="22"/>
+      <c r="H35" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="H35" s="31"/>
       <c r="I35" s="31"/>
-      <c r="J35" s="22"/>
+      <c r="J35" s="31"/>
       <c r="K35" s="22"/>
-    </row>
-    <row r="36" spans="1:12" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L35" s="22"/>
+    </row>
+    <row r="36" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="40" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E40" s="1"/>
     </row>
-    <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="L46" s="21"/>
-    </row>
-    <row r="55" spans="3:3" ht="15" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="46" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M46" s="21"/>
+    </row>
+    <row r="55" spans="3:3" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="59" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C59" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="A6:L7"/>
-    <mergeCell ref="A8:L8"/>
+  <mergeCells count="20">
+    <mergeCell ref="N15:N18"/>
+    <mergeCell ref="C27:M27"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="A6:M7"/>
+    <mergeCell ref="A8:M8"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="A26:F26"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="D13:E13"/>
-    <mergeCell ref="M15:M18"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="I9:L9"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="G19:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
+ Thêm số tiền bằng chữ (1 row below số tiền bằng số) + Sai giá trị field: File- AEL + Sai giá trị field: volumn (LCL: số khối, FCL: số cont)
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Tel : 848 - 62581123   Fax :  848 - 62581129</t>
   </si>
@@ -196,9 +196,6 @@
     <t>${custFax}</t>
   </si>
   <si>
-    <t>${aelcmb}</t>
-  </si>
-  <si>
     <t>${PTVT}</t>
   </si>
   <si>
@@ -338,6 +335,12 @@
   </si>
   <si>
     <t>${customFees.unitPrice}</t>
+  </si>
+  <si>
+    <t>${aelJob}</t>
+  </si>
+  <si>
+    <t>${totalText}</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -798,6 +801,21 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -861,20 +879,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="2" borderId="7" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1231,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView tabSelected="1" topLeftCell="C22" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1333,54 +1339,54 @@
       <c r="N5" s="35"/>
     </row>
     <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
       <c r="N6" s="36"/>
     </row>
     <row r="7" spans="1:14" ht="2.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="71"/>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
+      <c r="A7" s="76"/>
+      <c r="B7" s="76"/>
+      <c r="C7" s="76"/>
+      <c r="D7" s="76"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="H7" s="76"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
     </row>
     <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="72" t="s">
-        <v>56</v>
-      </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="72"/>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
+      <c r="A8" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="77"/>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77"/>
     </row>
     <row r="9" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="38"/>
@@ -1392,12 +1398,12 @@
       <c r="G9" s="68"/>
       <c r="H9" s="38"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="83" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
+      <c r="J9" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
     </row>
     <row r="10" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
@@ -1416,7 +1422,7 @@
         <v>18</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="M10" s="10"/>
     </row>
@@ -1437,7 +1443,7 @@
         <v>40</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M11" s="9"/>
     </row>
@@ -1458,7 +1464,7 @@
         <v>41</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M12" s="9"/>
     </row>
@@ -1472,10 +1478,10 @@
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="80" t="s">
+      <c r="D13" s="85" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="80"/>
+      <c r="E13" s="85"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
@@ -1501,54 +1507,54 @@
         <v>16</v>
       </c>
       <c r="B15" s="63" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="62"/>
       <c r="K15" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="L15" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="L15" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="N15" s="81"/>
+      <c r="N15" s="86"/>
     </row>
     <row r="16" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="89" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
+      <c r="E16" s="89"/>
+      <c r="F16" s="89"/>
       <c r="G16" s="67"/>
       <c r="H16" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>38</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="N16" s="81"/>
+        <v>53</v>
+      </c>
+      <c r="N16" s="86"/>
     </row>
     <row r="17" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="34"/>
@@ -1557,9 +1563,9 @@
         <v>39</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="N17" s="81"/>
+        <v>60</v>
+      </c>
+      <c r="N17" s="86"/>
     </row>
     <row r="18" spans="1:14" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="11"/>
@@ -1575,49 +1581,49 @@
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="32"/>
-      <c r="N18" s="81"/>
+      <c r="N18" s="86"/>
     </row>
     <row r="19" spans="1:14" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="78" t="s">
+      <c r="A19" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="78" t="s">
+      <c r="B19" s="83" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="85" t="s">
+      <c r="D19" s="90" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="86"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="90" t="s">
-        <v>95</v>
-      </c>
-      <c r="H19" s="88" t="s">
+      <c r="E19" s="91"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="95" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="78" t="s">
+      <c r="I19" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="78" t="s">
+      <c r="J19" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="78" t="s">
+      <c r="K19" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="L19" s="78" t="s">
+      <c r="L19" s="83" t="s">
         <v>25</v>
       </c>
-      <c r="M19" s="78" t="s">
+      <c r="M19" s="83" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="79"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="79"/>
+      <c r="A20" s="84"/>
+      <c r="B20" s="84"/>
+      <c r="C20" s="84"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1627,53 +1633,53 @@
       <c r="F20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="91"/>
-      <c r="H20" s="89"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="79"/>
-      <c r="K20" s="79"/>
-      <c r="L20" s="79"/>
-      <c r="M20" s="79"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="94"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
     </row>
     <row r="21" spans="1:14" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B21" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="D21" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="E21" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="F21" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="G21" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="H21" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="G21" s="92" t="s">
-        <v>96</v>
-      </c>
-      <c r="H21" s="93" t="s">
+      <c r="I21" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="I21" s="93" t="s">
+      <c r="J21" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="J21" s="93" t="s">
+      <c r="K21" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="K21" s="92" t="s">
+      <c r="L21" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="L21" s="59" t="s">
+      <c r="M21" s="59" t="s">
         <v>80</v>
-      </c>
-      <c r="M21" s="59" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1686,25 +1692,25 @@
       <c r="E22" s="58"/>
       <c r="F22" s="47"/>
       <c r="G22" s="47"/>
-      <c r="H22" s="95" t="s">
+      <c r="H22" s="74" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="49"/>
+      <c r="J22" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="95" t="s">
+      <c r="K22" s="74" t="s">
         <v>65</v>
-      </c>
-      <c r="K22" s="95" t="s">
-        <v>66</v>
       </c>
       <c r="L22" s="50"/>
       <c r="M22" s="50"/>
     </row>
     <row r="23" spans="1:14" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="73" t="s">
+      <c r="A23" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="74"/>
-      <c r="C23" s="74"/>
+      <c r="B23" s="79"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
@@ -1718,41 +1724,41 @@
     </row>
     <row r="24" spans="1:14" s="4" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="64" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="D24" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="D24" s="59" t="s">
+      <c r="E24" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="F24" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="59" t="s">
+      <c r="G24" s="59"/>
+      <c r="H24" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="93" t="s">
+      <c r="I24" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="I24" s="94" t="s">
+      <c r="J24" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="J24" s="93" t="s">
+      <c r="K24" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="K24" s="93" t="s">
+      <c r="L24" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="L24" s="60" t="s">
+      <c r="M24" s="60" t="s">
         <v>91</v>
-      </c>
-      <c r="M24" s="60" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -1765,28 +1771,28 @@
       <c r="E25" s="52"/>
       <c r="F25" s="53"/>
       <c r="G25" s="70"/>
-      <c r="H25" s="95" t="s">
+      <c r="H25" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="54"/>
+      <c r="J25" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="95" t="s">
-        <v>68</v>
-      </c>
-      <c r="K25" s="95" t="s">
-        <v>70</v>
+      <c r="K25" s="74" t="s">
+        <v>69</v>
       </c>
       <c r="L25" s="54"/>
       <c r="M25" s="55"/>
     </row>
     <row r="26" spans="1:14" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
-      <c r="F26" s="77"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="82"/>
       <c r="G26" s="69"/>
       <c r="H26" s="46"/>
       <c r="I26" s="44"/>
@@ -1798,17 +1804,17 @@
     <row r="27" spans="1:14" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="82"/>
-      <c r="E27" s="82"/>
-      <c r="F27" s="82"/>
-      <c r="G27" s="82"/>
-      <c r="H27" s="82"/>
-      <c r="I27" s="82"/>
-      <c r="J27" s="82"/>
-      <c r="K27" s="82"/>
-      <c r="L27" s="82"/>
-      <c r="M27" s="82"/>
+      <c r="C27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="87"/>
+      <c r="F27" s="87"/>
+      <c r="G27" s="87"/>
+      <c r="H27" s="87"/>
+      <c r="I27" s="87"/>
+      <c r="J27" s="87"/>
+      <c r="K27" s="87"/>
+      <c r="L27" s="87"/>
+      <c r="M27" s="87"/>
     </row>
     <row r="28" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="27" t="s">
@@ -1819,30 +1825,23 @@
       <c r="L28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="56" t="s">
+      <c r="M28" s="75" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="27"/>
+      <c r="B29" s="27"/>
+      <c r="D29" s="20"/>
+      <c r="K29" s="97" t="s">
+        <v>97</v>
+      </c>
+      <c r="L29" s="97"/>
+      <c r="M29" s="97"/>
+    </row>
+    <row r="30" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="56" t="s">
         <v>32</v>
-      </c>
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="13"/>
-    </row>
-    <row r="30" spans="1:14" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="56" t="s">
-        <v>33</v>
       </c>
       <c r="B30" s="56"/>
       <c r="C30" s="56"/>
@@ -1855,10 +1854,11 @@
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
-    </row>
-    <row r="31" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M30" s="13"/>
+    </row>
+    <row r="31" spans="1:14" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="56" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="56"/>
       <c r="C31" s="56"/>
@@ -1872,9 +1872,9 @@
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
     </row>
-    <row r="32" spans="1:14" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="56"/>
       <c r="C32" s="56"/>
@@ -1885,24 +1885,26 @@
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
       <c r="J32" s="28"/>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-    </row>
-    <row r="33" spans="1:13" ht="3" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="22"/>
-    </row>
-    <row r="34" spans="1:13" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+    </row>
+    <row r="33" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="56" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+    </row>
+    <row r="34" spans="1:13" ht="3" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="22"/>
@@ -1916,38 +1918,53 @@
       <c r="K34" s="22"/>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="31"/>
+    <row r="35" spans="1:13" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="30"/>
+      <c r="B35" s="30"/>
       <c r="C35" s="22"/>
       <c r="D35" s="22"/>
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
       <c r="G35" s="22"/>
-      <c r="H35" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
     </row>
-    <row r="36" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="E40" s="1"/>
-    </row>
-    <row r="42" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="46" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="M46" s="21"/>
-    </row>
-    <row r="55" spans="3:3" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="59" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C59" s="15"/>
+    <row r="36" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A36" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+    </row>
+    <row r="37" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="41" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="43" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M47" s="21"/>
+    </row>
+    <row r="56" spans="3:3" ht="14.5" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C60" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="21">
+    <mergeCell ref="K29:M29"/>
     <mergeCell ref="N15:N18"/>
     <mergeCell ref="C27:M27"/>
     <mergeCell ref="J9:M9"/>

</xml_diff>

<commit_message>
Fixed giá trị cho cột khác, tổng cộng 1+2 , ngày tờ khai
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Java\ael\src\main\resources\ExportTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="117" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
   <si>
     <t>Tel : 848 - 62581123   Fax :  848 - 62581129</t>
   </si>
@@ -217,9 +217,6 @@
     <t>Số : ${refNo}</t>
   </si>
   <si>
-    <t>Ngày: ${updateDate}</t>
-  </si>
-  <si>
     <t>HCM, ${updateDate}</t>
   </si>
   <si>
@@ -344,6 +341,21 @@
   </si>
   <si>
     <t>Số tiền bằng chữ</t>
+  </si>
+  <si>
+    <t>Khác</t>
+  </si>
+  <si>
+    <t>${customFees.numOfOther}</t>
+  </si>
+  <si>
+    <t>${thanhtienTong}</t>
+  </si>
+  <si>
+    <t>${tongcongTong}</t>
+  </si>
+  <si>
+    <t>Ngày: ${customsDate}</t>
   </si>
 </sst>
 </file>
@@ -652,7 +664,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -816,6 +828,66 @@
     <xf numFmtId="3" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -837,58 +909,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="9" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="20" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1246,92 +1267,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="24.54296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.7265625" style="17" customWidth="1"/>
-    <col min="5" max="7" width="5.81640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="12.453125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="14.7265625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="22.453125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16" style="2" customWidth="1"/>
-    <col min="14" max="14" width="21.1796875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="9" style="2"/>
+    <col min="1" max="1" width="14.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="17" customWidth="1"/>
+    <col min="5" max="8" width="5.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="16" style="2" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="H1" s="22"/>
+    <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I1" s="22"/>
-      <c r="M1" s="40" t="s">
+      <c r="J1" s="22"/>
+      <c r="N1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="23"/>
-    </row>
-    <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O1" s="23"/>
+    </row>
+    <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="18"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="7"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="24"/>
+      <c r="H2" s="7"/>
       <c r="I2" s="24"/>
-      <c r="J2" s="7"/>
+      <c r="J2" s="24"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="M2" s="41" t="s">
+      <c r="M2" s="7"/>
+      <c r="N2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="25"/>
-    </row>
-    <row r="3" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O2" s="25"/>
+    </row>
+    <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="18"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="24"/>
+      <c r="H3" s="7"/>
       <c r="I3" s="24"/>
-      <c r="J3" s="7"/>
+      <c r="J3" s="24"/>
       <c r="K3" s="7"/>
       <c r="L3" s="7"/>
-      <c r="M3" s="41" t="s">
+      <c r="M3" s="7"/>
+      <c r="N3" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="25"/>
-    </row>
-    <row r="4" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="O3" s="25"/>
+    </row>
+    <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="18"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="7"/>
-      <c r="H4" s="24"/>
+      <c r="H4" s="7"/>
       <c r="I4" s="24"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="24"/>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
-      <c r="M4" s="41" t="s">
+      <c r="M4" s="7"/>
+      <c r="N4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="25"/>
-    </row>
-    <row r="5" spans="1:14" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="25"/>
+    </row>
+    <row r="5" spans="1:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="14"/>
@@ -1339,82 +1363,87 @@
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
-      <c r="H5" s="26"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="26"/>
       <c r="J5" s="26"/>
       <c r="K5" s="26"/>
       <c r="L5" s="26"/>
       <c r="M5" s="26"/>
-      <c r="N5" s="35"/>
-    </row>
-    <row r="6" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="75" t="s">
+      <c r="N5" s="26"/>
+      <c r="O5" s="35"/>
+    </row>
+    <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="36"/>
-    </row>
-    <row r="7" spans="1:14" ht="2.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="75"/>
-      <c r="B7" s="75"/>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="75"/>
-      <c r="K7" s="75"/>
-      <c r="L7" s="75"/>
-      <c r="M7" s="75"/>
-    </row>
-    <row r="8" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="76" t="s">
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="95"/>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="95"/>
+      <c r="O6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="95"/>
+      <c r="B7" s="95"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="95"/>
+      <c r="H7" s="95"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="95"/>
+      <c r="K7" s="95"/>
+      <c r="L7" s="95"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="95"/>
+    </row>
+    <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-      <c r="I8" s="76"/>
-      <c r="J8" s="76"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="76"/>
-      <c r="M8" s="76"/>
-    </row>
-    <row r="9" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="96"/>
+      <c r="C8" s="96"/>
+      <c r="D8" s="96"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="96"/>
+    </row>
+    <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
       <c r="D9" s="38"/>
       <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="38"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="68"/>
       <c r="I9" s="38"/>
-      <c r="J9" s="88" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="88"/>
-      <c r="L9" s="88"/>
-      <c r="M9" s="88"/>
-    </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J9" s="38"/>
+      <c r="K9" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="83"/>
+      <c r="M9" s="83"/>
+      <c r="N9" s="83"/>
+    </row>
+    <row r="10" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -1424,18 +1453,19 @@
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
-      <c r="H10" s="10"/>
+      <c r="F10" s="77"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M10" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="N10" s="10"/>
+    </row>
+    <row r="11" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>13</v>
       </c>
@@ -1445,18 +1475,19 @@
       <c r="C11" s="39"/>
       <c r="D11" s="9"/>
       <c r="E11" s="39"/>
-      <c r="H11" s="9"/>
+      <c r="F11" s="77"/>
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="9"/>
+      <c r="L11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L11" s="9" t="s">
+      <c r="M11" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>14</v>
       </c>
@@ -1466,18 +1497,19 @@
       <c r="C12" s="39"/>
       <c r="D12" s="9"/>
       <c r="E12" s="39"/>
-      <c r="H12" s="9"/>
+      <c r="F12" s="77"/>
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="9"/>
+      <c r="L12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="L12" s="9" t="s">
+      <c r="M12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -1487,78 +1519,82 @@
       <c r="C13" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="84" t="s">
+      <c r="D13" s="102" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="84"/>
-      <c r="H13" s="9"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="76"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
-    </row>
-    <row r="14" spans="1:14" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:15" s="3" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="33"/>
       <c r="C14" s="57"/>
       <c r="D14" s="10"/>
       <c r="E14" s="57"/>
-      <c r="H14" s="9"/>
+      <c r="F14" s="77"/>
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-    </row>
-    <row r="15" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N14" s="9"/>
+    </row>
+    <row r="15" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B15" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>59</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="62"/>
-      <c r="K15" s="9" t="s">
+      <c r="F15" s="77"/>
+      <c r="L15" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L15" s="33" t="s">
+      <c r="M15" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="N15" s="86"/>
-    </row>
-    <row r="16" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O15" s="81"/>
+    </row>
+    <row r="16" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D16" s="84" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="67"/>
+      <c r="I16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="89" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="89"/>
-      <c r="F16" s="89"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="K16" s="9" t="s">
+      <c r="L16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L16" s="33" t="s">
+      <c r="M16" s="33" t="s">
         <v>53</v>
       </c>
-      <c r="N16" s="86"/>
-    </row>
-    <row r="17" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O16" s="81"/>
+    </row>
+    <row r="17" spans="1:15" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>43</v>
       </c>
@@ -1568,71 +1604,74 @@
       <c r="C17" s="16"/>
       <c r="D17" s="34"/>
       <c r="E17" s="39"/>
-      <c r="K17" s="9" t="s">
+      <c r="F17" s="77"/>
+      <c r="L17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L17" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="N17" s="86"/>
-    </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M17" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="O17" s="81"/>
+    </row>
+    <row r="18" spans="1:15" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="11"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="66"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="32"/>
-      <c r="N18" s="86"/>
-    </row>
-    <row r="19" spans="1:14" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="82" t="s">
+      <c r="M18" s="9"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="81"/>
+    </row>
+    <row r="19" spans="1:15" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="90" t="s">
+      <c r="D19" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="91"/>
-      <c r="F19" s="92"/>
-      <c r="G19" s="95" t="s">
-        <v>94</v>
-      </c>
-      <c r="H19" s="93" t="s">
+      <c r="E19" s="88"/>
+      <c r="F19" s="88"/>
+      <c r="G19" s="89"/>
+      <c r="H19" s="92" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="90" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="82" t="s">
+      <c r="J19" s="85" t="s">
         <v>22</v>
       </c>
-      <c r="J19" s="82" t="s">
+      <c r="K19" s="85" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="82" t="s">
+      <c r="L19" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="L19" s="82" t="s">
+      <c r="M19" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="M19" s="82" t="s">
+      <c r="N19" s="85" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="83"/>
-      <c r="B20" s="83"/>
-      <c r="C20" s="83"/>
+    <row r="20" spans="1:15" s="4" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="86"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="12" t="s">
         <v>3</v>
       </c>
@@ -1640,58 +1679,64 @@
         <v>4</v>
       </c>
       <c r="F20" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="G20" s="96"/>
-      <c r="H20" s="94"/>
-      <c r="I20" s="83"/>
-      <c r="J20" s="83"/>
-      <c r="K20" s="83"/>
-      <c r="L20" s="83"/>
-      <c r="M20" s="83"/>
-    </row>
-    <row r="21" spans="1:14" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H20" s="93"/>
+      <c r="I20" s="91"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="86"/>
+      <c r="N20" s="86"/>
+    </row>
+    <row r="21" spans="1:15" s="4" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="64" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B21" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="64" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="64" t="s">
+      <c r="D21" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="E21" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="E21" s="59" t="s">
+      <c r="F21" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="G21" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="F21" s="59" t="s">
+      <c r="H21" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="I21" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="G21" s="74" t="s">
-        <v>95</v>
-      </c>
-      <c r="H21" s="73" t="s">
+      <c r="J21" s="78" t="s">
         <v>75</v>
       </c>
-      <c r="I21" s="97" t="s">
+      <c r="K21" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="J21" s="73" t="s">
+      <c r="L21" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="K21" s="74" t="s">
+      <c r="M21" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="L21" s="59" t="s">
+      <c r="N21" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="M21" s="59" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:15" s="4" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="47"/>
       <c r="C22" s="48" t="s">
@@ -1699,27 +1744,28 @@
       </c>
       <c r="D22" s="58"/>
       <c r="E22" s="58"/>
-      <c r="F22" s="47"/>
+      <c r="F22" s="58"/>
       <c r="G22" s="47"/>
-      <c r="H22" s="72" t="s">
+      <c r="H22" s="47"/>
+      <c r="I22" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" s="49"/>
+      <c r="K22" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="49"/>
-      <c r="J22" s="72" t="s">
+      <c r="L22" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="K22" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="L22" s="50"/>
       <c r="M22" s="50"/>
-    </row>
-    <row r="23" spans="1:14" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="77" t="s">
+      <c r="N22" s="50"/>
+    </row>
+    <row r="23" spans="1:15" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="97" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="78"/>
-      <c r="C23" s="78"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="98"/>
       <c r="D23" s="42"/>
       <c r="E23" s="42"/>
       <c r="F23" s="42"/>
@@ -1729,48 +1775,50 @@
       <c r="J23" s="42"/>
       <c r="K23" s="42"/>
       <c r="L23" s="42"/>
-      <c r="M23" s="43"/>
-    </row>
-    <row r="24" spans="1:14" s="4" customFormat="1" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M23" s="42"/>
+      <c r="N23" s="43"/>
+    </row>
+    <row r="24" spans="1:15" s="4" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="64" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B24" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="65" t="s">
         <v>81</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="D24" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="D24" s="59" t="s">
+      <c r="E24" s="59" t="s">
         <v>83</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="F24" s="59"/>
+      <c r="G24" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="F24" s="59" t="s">
+      <c r="H24" s="59"/>
+      <c r="I24" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="G24" s="59"/>
-      <c r="H24" s="73" t="s">
+      <c r="J24" s="79" t="s">
         <v>86</v>
       </c>
-      <c r="I24" s="98" t="s">
+      <c r="K24" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="J24" s="73" t="s">
+      <c r="L24" s="73" t="s">
         <v>88</v>
       </c>
-      <c r="K24" s="73" t="s">
+      <c r="M24" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="L24" s="60" t="s">
+      <c r="N24" s="60" t="s">
         <v>90</v>
       </c>
-      <c r="M24" s="60" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:15" s="5" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="51"/>
       <c r="B25" s="52"/>
       <c r="C25" s="51" t="s">
@@ -1778,79 +1826,88 @@
       </c>
       <c r="D25" s="52"/>
       <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
-      <c r="G25" s="70"/>
-      <c r="H25" s="72" t="s">
+      <c r="F25" s="52"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="70"/>
+      <c r="I25" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="54"/>
+      <c r="K25" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="K25" s="72" t="s">
-        <v>69</v>
-      </c>
-      <c r="L25" s="54"/>
-      <c r="M25" s="55"/>
-    </row>
-    <row r="26" spans="1:14" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="79" t="s">
+      <c r="L25" s="72" t="s">
+        <v>68</v>
+      </c>
+      <c r="M25" s="54"/>
+      <c r="N25" s="55"/>
+    </row>
+    <row r="26" spans="1:15" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="80"/>
-      <c r="C26" s="80"/>
-      <c r="D26" s="80"/>
-      <c r="E26" s="80"/>
-      <c r="F26" s="81"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="46"/>
+      <c r="B26" s="100"/>
+      <c r="C26" s="100"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="100"/>
+      <c r="F26" s="100"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="J26" s="44"/>
       <c r="K26" s="46"/>
-      <c r="L26" s="44"/>
+      <c r="L26" s="46" t="s">
+        <v>101</v>
+      </c>
       <c r="M26" s="44"/>
-    </row>
-    <row r="27" spans="1:14" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="N26" s="44"/>
+    </row>
+    <row r="27" spans="1:15" s="5" customFormat="1" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="27"/>
       <c r="B27" s="27"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
-      <c r="I27" s="87"/>
-      <c r="J27" s="87"/>
-      <c r="K27" s="87"/>
-      <c r="L27" s="87"/>
-      <c r="M27" s="87"/>
-    </row>
-    <row r="28" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="82"/>
+      <c r="D27" s="82"/>
+      <c r="E27" s="82"/>
+      <c r="F27" s="82"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="82"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="82"/>
+      <c r="L27" s="82"/>
+      <c r="M27" s="82"/>
+      <c r="N27" s="82"/>
+    </row>
+    <row r="28" spans="1:15" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="27"/>
       <c r="D28" s="20"/>
-      <c r="L28" s="45" t="s">
+      <c r="M28" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="M28" s="71" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="99" t="s">
-        <v>98</v>
-      </c>
-      <c r="B29" s="99"/>
+      <c r="N28" s="71" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="80" t="s">
+        <v>97</v>
+      </c>
+      <c r="B29" s="80"/>
       <c r="D29" s="20"/>
-      <c r="K29" s="85" t="s">
-        <v>97</v>
-      </c>
-      <c r="L29" s="85"/>
-      <c r="M29" s="85"/>
-    </row>
-    <row r="30" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J29" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="K29" s="94"/>
+      <c r="L29" s="94"/>
+      <c r="M29" s="94"/>
+      <c r="N29" s="94"/>
+    </row>
+    <row r="30" spans="1:15" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="56" t="s">
         <v>32</v>
       </c>
@@ -1860,14 +1917,15 @@
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
-      <c r="H30" s="28"/>
+      <c r="H30" s="13"/>
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
-      <c r="M30" s="13"/>
-    </row>
-    <row r="31" spans="1:14" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M30" s="28"/>
+      <c r="N30" s="13"/>
+    </row>
+    <row r="31" spans="1:15" s="5" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="56" t="s">
         <v>33</v>
       </c>
@@ -1877,13 +1935,14 @@
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
-      <c r="H31" s="28"/>
+      <c r="H31" s="13"/>
       <c r="I31" s="28"/>
       <c r="J31" s="28"/>
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
-    </row>
-    <row r="32" spans="1:14" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M31" s="28"/>
+    </row>
+    <row r="32" spans="1:15" s="5" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="56" t="s">
         <v>34</v>
       </c>
@@ -1893,13 +1952,14 @@
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
-      <c r="H32" s="28"/>
+      <c r="H32" s="13"/>
       <c r="I32" s="28"/>
       <c r="J32" s="28"/>
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
-    </row>
-    <row r="33" spans="1:13" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M32" s="28"/>
+    </row>
+    <row r="33" spans="1:14" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="56" t="s">
         <v>35</v>
       </c>
@@ -1909,13 +1969,14 @@
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
-      <c r="H33" s="28"/>
+      <c r="H33" s="13"/>
       <c r="I33" s="28"/>
       <c r="J33" s="28"/>
-      <c r="K33" s="29"/>
+      <c r="K33" s="28"/>
       <c r="L33" s="29"/>
-    </row>
-    <row r="34" spans="1:13" ht="3" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M33" s="29"/>
+    </row>
+    <row r="34" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="22"/>
@@ -1928,8 +1989,9 @@
       <c r="J34" s="22"/>
       <c r="K34" s="22"/>
       <c r="L34" s="22"/>
-    </row>
-    <row r="35" spans="1:13" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M34" s="22"/>
+    </row>
+    <row r="35" spans="1:14" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="22"/>
@@ -1942,8 +2004,9 @@
       <c r="J35" s="22"/>
       <c r="K35" s="22"/>
       <c r="L35" s="22"/>
-    </row>
-    <row r="36" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="M35" s="22"/>
+    </row>
+    <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
         <v>7</v>
       </c>
@@ -1953,50 +2016,52 @@
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
       <c r="G36" s="22"/>
-      <c r="H36" s="31" t="s">
+      <c r="H36" s="22"/>
+      <c r="I36" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="I36" s="31"/>
       <c r="J36" s="31"/>
-      <c r="K36" s="22"/>
+      <c r="K36" s="31"/>
       <c r="L36" s="22"/>
-    </row>
-    <row r="37" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="41" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M36" s="22"/>
+    </row>
+    <row r="37" spans="1:14" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="1"/>
-    </row>
-    <row r="43" spans="1:13" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="47" spans="1:13" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="M47" s="21"/>
-    </row>
-    <row r="56" spans="3:3" ht="14.5" x14ac:dyDescent="0.35"/>
-    <row r="60" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F41" s="1"/>
+    </row>
+    <row r="43" spans="1:14" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N47" s="21"/>
+    </row>
+    <row r="56" spans="3:3" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C60" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="K29:M29"/>
-    <mergeCell ref="N15:N18"/>
-    <mergeCell ref="C27:M27"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="A6:M7"/>
-    <mergeCell ref="A8:M8"/>
+    <mergeCell ref="A6:N7"/>
+    <mergeCell ref="A8:N8"/>
     <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A26:G26"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="O15:O18"/>
+    <mergeCell ref="C27:N27"/>
+    <mergeCell ref="K9:N9"/>
+    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:G19"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="J29:N29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
chi phi trung : done 4. sua debit : done 6. Noi lay cont noi ha cont 7. xe lai bang ke nha thau : work explain 8. duyet chi phi trucking + them so cont : done 9. Them nha thau error => ok
</commit_message>
<xml_diff>
--- a/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
+++ b/src/main/resources/ExportTemplate/DebitNoteTemplate.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\src\main\resources\ExportTemplate\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
   <si>
     <t>Tel : 848 - 62581123   Fax :  848 - 62581129</t>
   </si>
@@ -349,6 +354,12 @@
       </rPr>
       <t>103714189</t>
     </r>
+  </si>
+  <si>
+    <t>Nơi giao hàng:</t>
+  </si>
+  <si>
+    <t>${delivery}</t>
   </si>
 </sst>
 </file>
@@ -600,16 +611,7 @@
     <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -623,9 +625,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -635,46 +634,15 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -691,12 +659,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -720,15 +682,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -736,20 +689,11 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="4" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -783,6 +727,75 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="6" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -894,7 +907,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -929,7 +942,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1140,430 +1153,436 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="55" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" style="55" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" style="55" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="64" customWidth="1"/>
-    <col min="5" max="8" width="5.85546875" style="55" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="55" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="55" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="55" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" style="55" customWidth="1"/>
-    <col min="13" max="13" width="22.42578125" style="55" customWidth="1"/>
-    <col min="14" max="14" width="16" style="55" customWidth="1"/>
-    <col min="15" max="15" width="21.140625" style="55" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="55"/>
+    <col min="1" max="1" width="14.42578125" style="38" customWidth="1"/>
+    <col min="2" max="2" width="24.7109375" style="38" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="5.7109375" style="43" customWidth="1"/>
+    <col min="5" max="8" width="5.85546875" style="38" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="38" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="38" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" style="38" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="38" customWidth="1"/>
+    <col min="13" max="13" width="22.42578125" style="38" customWidth="1"/>
+    <col min="14" max="14" width="16" style="38" customWidth="1"/>
+    <col min="15" max="15" width="21.140625" style="38" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="N1" s="75" t="s">
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="N1" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="76"/>
+      <c r="O1" s="53"/>
     </row>
     <row r="2" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="70"/>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="78" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="47"/>
+      <c r="N2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="79"/>
+      <c r="O2" s="56"/>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70"/>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="78" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="47"/>
+      <c r="M3" s="47"/>
+      <c r="N3" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="O3" s="79"/>
+      <c r="O3" s="56"/>
     </row>
     <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70"/>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="70"/>
-      <c r="L4" s="70"/>
-      <c r="M4" s="70"/>
-      <c r="N4" s="78" t="s">
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="47"/>
+      <c r="N4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="O4" s="79"/>
+      <c r="O4" s="56"/>
     </row>
     <row r="5" spans="1:15" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="70"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="82"/>
-      <c r="K5" s="82"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
-      <c r="N5" s="82"/>
-      <c r="O5" s="83"/>
+      <c r="A5" s="47"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="58"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="60"/>
     </row>
     <row r="6" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="64" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="17"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
+      <c r="J6" s="64"/>
+      <c r="K6" s="64"/>
+      <c r="L6" s="64"/>
+      <c r="M6" s="64"/>
+      <c r="N6" s="64"/>
+      <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
     </row>
     <row r="9" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-    </row>
-    <row r="10" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="76"/>
+    </row>
+    <row r="10" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="18" t="s">
+      <c r="M10" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="N10" s="18"/>
-    </row>
-    <row r="11" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="N10" s="15"/>
+    </row>
+    <row r="11" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19" t="s">
+      <c r="C11" s="13"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="M11" s="19" t="s">
+      <c r="M11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="19"/>
-    </row>
-    <row r="12" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="N11" s="16"/>
+    </row>
+    <row r="12" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19" t="s">
+      <c r="C12" s="13"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M12" s="19" t="s">
+      <c r="M12" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N12" s="19"/>
-    </row>
-    <row r="13" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="N12" s="16"/>
+    </row>
+    <row r="13" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="20"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19"/>
-    </row>
-    <row r="14" spans="1:15" s="17" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19"/>
-    </row>
-    <row r="15" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="E13" s="72"/>
+      <c r="F13" s="17"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="16"/>
+      <c r="N13" s="16"/>
+    </row>
+    <row r="14" spans="1:15" s="14" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="16"/>
+      <c r="N14" s="16"/>
+    </row>
+    <row r="15" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="19"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="L15" s="19" t="s">
+      <c r="D15" s="16"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="L15" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="M15" s="20" t="s">
+      <c r="M15" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="O15" s="10"/>
-    </row>
-    <row r="16" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="O15" s="74"/>
+    </row>
+    <row r="16" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="D16" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="17" t="s">
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="L16" s="19" t="s">
+      <c r="L16" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="M16" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="O16" s="10"/>
-    </row>
-    <row r="17" spans="1:15" s="17" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="O16" s="74"/>
+    </row>
+    <row r="17" spans="1:15" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="L17" s="19" t="s">
+      <c r="C17" s="12"/>
+      <c r="D17" s="86" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="I17" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="L17" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="M17" s="18" t="s">
+      <c r="M17" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="10"/>
-    </row>
-    <row r="18" spans="1:15" s="17" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="10"/>
-    </row>
-    <row r="19" spans="1:15" s="34" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="28" t="s">
+      <c r="O17" s="74"/>
+    </row>
+    <row r="18" spans="1:15" s="14" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="16"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="74"/>
+    </row>
+    <row r="19" spans="1:15" s="22" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="70" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="70" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D19" s="78" t="s">
         <v>2</v>
       </c>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32" t="s">
+      <c r="E19" s="79"/>
+      <c r="F19" s="79"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="33" t="s">
+      <c r="I19" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="J19" s="28" t="s">
+      <c r="J19" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="K19" s="28" t="s">
+      <c r="K19" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="L19" s="28" t="s">
+      <c r="L19" s="70" t="s">
         <v>24</v>
       </c>
-      <c r="M19" s="28" t="s">
+      <c r="M19" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="N19" s="28" t="s">
+      <c r="N19" s="70" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="34" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="36" t="s">
+    <row r="20" spans="1:15" s="22" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="71"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="36" t="s">
+      <c r="E20" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="36" t="s">
+      <c r="G20" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-    </row>
-    <row r="21" spans="1:15" s="34" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H20" s="84"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="71"/>
+      <c r="K20" s="71"/>
+      <c r="L20" s="71"/>
+      <c r="M20" s="71"/>
+      <c r="N20" s="71"/>
+    </row>
+    <row r="21" spans="1:15" s="22" customFormat="1" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>89</v>
       </c>
@@ -1607,49 +1626,49 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:15" s="34" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="40" t="s">
+    <row r="22" spans="1:15" s="22" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="42" t="s">
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="J22" s="43"/>
-      <c r="K22" s="42" t="s">
+      <c r="J22" s="28"/>
+      <c r="K22" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="L22" s="42" t="s">
+      <c r="L22" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="M22" s="44"/>
-      <c r="N22" s="44"/>
-    </row>
-    <row r="23" spans="1:15" s="34" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="45" t="s">
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" s="22" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="65" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
-      <c r="L23" s="47"/>
-      <c r="M23" s="47"/>
-      <c r="N23" s="48"/>
-    </row>
-    <row r="24" spans="1:15" s="34" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="66"/>
+      <c r="C23" s="66"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+      <c r="J23" s="30"/>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" s="22" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>90</v>
       </c>
@@ -1690,232 +1709,225 @@
       </c>
     </row>
     <row r="25" spans="1:15" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="49"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="49" t="s">
+      <c r="A25" s="32"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="52"/>
-      <c r="I25" s="42" t="s">
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="J25" s="53"/>
-      <c r="K25" s="42" t="s">
+      <c r="J25" s="36"/>
+      <c r="K25" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="L25" s="42" t="s">
+      <c r="L25" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="M25" s="53"/>
-      <c r="N25" s="54"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="37"/>
     </row>
     <row r="26" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="60" t="s">
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="40" t="s">
         <v>98</v>
       </c>
-      <c r="J26" s="61"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60" t="s">
+      <c r="J26" s="41"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40" t="s">
         <v>99</v>
       </c>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
     </row>
     <row r="27" spans="1:15" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
-      <c r="I27" s="63"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="63"/>
-      <c r="L27" s="63"/>
-      <c r="M27" s="63"/>
-      <c r="N27" s="63"/>
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
+      <c r="J27" s="75"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="75"/>
+      <c r="M27" s="75"/>
+      <c r="N27" s="75"/>
     </row>
     <row r="28" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="62"/>
-      <c r="M28" s="65" t="s">
+      <c r="B28" s="42"/>
+      <c r="M28" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="N28" s="66" t="s">
+      <c r="N28" s="45" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="67" t="s">
+      <c r="A29" s="73" t="s">
         <v>95</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="J29" s="68" t="s">
+      <c r="B29" s="73"/>
+      <c r="J29" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="68"/>
-      <c r="N29" s="68"/>
+      <c r="K29" s="85"/>
+      <c r="L29" s="85"/>
+      <c r="M29" s="85"/>
+      <c r="N29" s="85"/>
     </row>
     <row r="30" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="69" t="s">
+      <c r="A30" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="70"/>
-      <c r="F30" s="70"/>
-      <c r="G30" s="70"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="71"/>
-      <c r="L30" s="71"/>
-      <c r="M30" s="71"/>
-      <c r="N30" s="70"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="48"/>
+      <c r="K30" s="48"/>
+      <c r="L30" s="48"/>
+      <c r="M30" s="48"/>
+      <c r="N30" s="47"/>
     </row>
     <row r="31" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="69" t="s">
+      <c r="A31" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="70"/>
-      <c r="F31" s="70"/>
-      <c r="G31" s="70"/>
-      <c r="H31" s="70"/>
-      <c r="I31" s="71"/>
-      <c r="J31" s="71"/>
-      <c r="K31" s="71"/>
-      <c r="L31" s="71"/>
-      <c r="M31" s="71"/>
+      <c r="B31" s="46"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
     </row>
     <row r="32" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="69" t="s">
+      <c r="A32" s="46" t="s">
         <v>102</v>
       </c>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="70"/>
-      <c r="F32" s="70"/>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="71"/>
-      <c r="J32" s="71"/>
-      <c r="K32" s="71"/>
-      <c r="L32" s="71"/>
-      <c r="M32" s="71"/>
+      <c r="B32" s="46"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="48"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="48"/>
+      <c r="L32" s="48"/>
+      <c r="M32" s="48"/>
     </row>
     <row r="33" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="69" t="s">
+      <c r="A33" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="70"/>
-      <c r="G33" s="70"/>
-      <c r="H33" s="70"/>
-      <c r="I33" s="71"/>
-      <c r="J33" s="71"/>
-      <c r="K33" s="71"/>
-      <c r="L33" s="72"/>
-      <c r="M33" s="72"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="48"/>
+      <c r="J33" s="48"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
     </row>
     <row r="34" spans="1:14" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="73"/>
-      <c r="B34" s="73"/>
-      <c r="C34" s="74"/>
-      <c r="D34" s="74"/>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="74"/>
-      <c r="J34" s="74"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="74"/>
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="51"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="51"/>
+      <c r="K34" s="51"/>
+      <c r="L34" s="51"/>
+      <c r="M34" s="51"/>
     </row>
     <row r="35" spans="1:14" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="73"/>
-      <c r="B35" s="73"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="74"/>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
+      <c r="A35" s="50"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="51"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
     </row>
     <row r="36" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="84" t="s">
+      <c r="A36" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="84"/>
-      <c r="C36" s="74"/>
-      <c r="D36" s="74"/>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74"/>
-      <c r="I36" s="84" t="s">
+      <c r="B36" s="61"/>
+      <c r="C36" s="51"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="51"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="J36" s="84"/>
-      <c r="K36" s="84"/>
-      <c r="L36" s="74"/>
-      <c r="M36" s="74"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="61"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
     </row>
     <row r="37" spans="1:14" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="41" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E41" s="65"/>
-      <c r="F41" s="65"/>
+      <c r="E41" s="44"/>
+      <c r="F41" s="44"/>
     </row>
     <row r="43" spans="1:14" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N47" s="85"/>
+      <c r="N47" s="62"/>
     </row>
     <row r="56" spans="3:3" ht="15.75" x14ac:dyDescent="0.25"/>
     <row r="60" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C60" s="86"/>
+      <c r="C60" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="A6:N7"/>
-    <mergeCell ref="A8:N8"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D13:E13"/>
+  <mergeCells count="23">
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="O15:O18"/>
     <mergeCell ref="C27:N27"/>
@@ -1931,6 +1943,14 @@
     <mergeCell ref="I19:I20"/>
     <mergeCell ref="H19:H20"/>
     <mergeCell ref="J29:N29"/>
+    <mergeCell ref="D17:G17"/>
+    <mergeCell ref="A6:N7"/>
+    <mergeCell ref="A8:N8"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="75" orientation="landscape" r:id="rId1"/>

</xml_diff>